<commit_message>
Notes on grid runs
</commit_message>
<xml_diff>
--- a/2028_07_28_grid_runs.xlsx
+++ b/2028_07_28_grid_runs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ofp-sam\yft-2023-grid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C20BEC3-F717-4EBA-8CD9-F35C617E86E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0F77EC-084F-4F03-B0AD-3BE181821DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{3B6CBC9F-90F2-4494-87E4-5FC31562FACF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="85">
   <si>
     <t>14a_par</t>
   </si>
@@ -237,6 +237,60 @@
   </si>
   <si>
     <t>in 11</t>
+  </si>
+  <si>
+    <t>dir</t>
+  </si>
+  <si>
+    <t>job.id</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>submit.time</t>
+  </si>
+  <si>
+    <t>runtime</t>
+  </si>
+  <si>
+    <t>disk</t>
+  </si>
+  <si>
+    <t>memory</t>
+  </si>
+  <si>
+    <t>14a_m2_s20_a075_h80</t>
+  </si>
+  <si>
+    <t>finished</t>
+  </si>
+  <si>
+    <t>14c_m2_s20_a075_h95</t>
+  </si>
+  <si>
+    <t>14a_m2_s20_a075_h65</t>
+  </si>
+  <si>
+    <t>14a_m2_s20_a075_h95</t>
+  </si>
+  <si>
+    <t>14c_m2_s20_a100_h65</t>
+  </si>
+  <si>
+    <t>14a_m2_s20_a100_h80</t>
+  </si>
+  <si>
+    <t>14a_m2_s20_a100_h95</t>
+  </si>
+  <si>
+    <t>14a_m2_s20_a100_h65</t>
+  </si>
+  <si>
+    <t>submit.date</t>
+  </si>
+  <si>
+    <t>diagnostic</t>
   </si>
 </sst>
 </file>
@@ -286,9 +340,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,356 +659,586 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFDE747-9AAB-4DFA-9C43-CC70659712BF}">
-  <dimension ref="B2:N30"/>
+  <dimension ref="A2:R30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
+        <v>67</v>
+      </c>
       <c r="L2" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="M2" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="N2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+      <c r="O2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="J4" t="s">
+      <c r="J3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K3" t="s">
+        <v>74</v>
+      </c>
+      <c r="L3">
+        <v>204256</v>
+      </c>
+      <c r="M3" t="s">
+        <v>75</v>
+      </c>
+      <c r="N3" s="2">
+        <v>46935</v>
+      </c>
+      <c r="O3" s="3">
+        <v>2.2754629629629628E-2</v>
+      </c>
+      <c r="P3" s="3">
+        <v>5.5555555555555556E-4</v>
+      </c>
+      <c r="Q3">
+        <v>325</v>
+      </c>
+      <c r="R3">
+        <v>5105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="L4" t="s">
+      <c r="F4" t="s">
         <v>34</v>
       </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" t="s">
+        <v>76</v>
+      </c>
+      <c r="L4">
+        <v>204284</v>
+      </c>
       <c r="M4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+      <c r="N4" s="2">
+        <v>46935</v>
+      </c>
+      <c r="O4" s="3">
+        <v>4.0902777777777781E-2</v>
+      </c>
+      <c r="P4" s="3">
+        <v>6.5277777777777782E-3</v>
+      </c>
+      <c r="Q4">
+        <v>328</v>
+      </c>
+      <c r="R4">
+        <v>5238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
       <c r="B5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" t="s">
         <v>65</v>
       </c>
-      <c r="J5" t="s">
+      <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="L5" t="s">
+      <c r="F5" t="s">
         <v>35</v>
       </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" t="s">
+        <v>77</v>
+      </c>
+      <c r="L5">
+        <v>204255</v>
+      </c>
       <c r="M5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+      <c r="N5" s="2">
+        <v>46935</v>
+      </c>
+      <c r="O5" s="3">
+        <v>2.269675925925926E-2</v>
+      </c>
+      <c r="P5" s="3">
+        <v>9.6064814814814815E-3</v>
+      </c>
+      <c r="Q5">
+        <v>328</v>
+      </c>
+      <c r="R5">
+        <v>5109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
       <c r="B6" t="s">
         <v>63</v>
       </c>
-      <c r="C6" t="s">
-        <v>63</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="L6" t="s">
+      <c r="F6" t="s">
         <v>36</v>
       </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" t="s">
+        <v>78</v>
+      </c>
+      <c r="L6">
+        <v>204257</v>
+      </c>
       <c r="M6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+      <c r="N6" s="2">
+        <v>46935</v>
+      </c>
+      <c r="O6" s="3">
+        <v>2.2824074074074076E-2</v>
+      </c>
+      <c r="P6" s="3">
+        <v>1.2777777777777777E-2</v>
+      </c>
+      <c r="Q6">
+        <v>328</v>
+      </c>
+      <c r="R6">
+        <v>5244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
       <c r="B7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" t="s">
         <v>66</v>
       </c>
-      <c r="J7" t="s">
+      <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="L7" t="s">
+      <c r="F7" t="s">
         <v>37</v>
       </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L7">
+        <v>204285</v>
+      </c>
       <c r="M7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="J8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N7" s="2">
+        <v>46935</v>
+      </c>
+      <c r="O7" s="3">
+        <v>4.0960648148148149E-2</v>
+      </c>
+      <c r="P7" s="3">
+        <v>3.9618055555555552E-2</v>
+      </c>
+      <c r="Q7">
+        <v>329</v>
+      </c>
+      <c r="R7">
+        <v>5239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="L8" t="s">
+      <c r="F8" t="s">
         <v>38</v>
       </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" t="s">
+        <v>80</v>
+      </c>
+      <c r="L8">
+        <v>204259</v>
+      </c>
       <c r="M8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="J9" t="s">
+        <v>75</v>
+      </c>
+      <c r="N8" s="2">
+        <v>46935</v>
+      </c>
+      <c r="O8" s="3">
+        <v>2.2962962962962966E-2</v>
+      </c>
+      <c r="P8" s="3">
+        <v>7.7534722222222227E-2</v>
+      </c>
+      <c r="Q8">
+        <v>330</v>
+      </c>
+      <c r="R8">
+        <v>5245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="L9" t="s">
+      <c r="F9" t="s">
         <v>39</v>
       </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" t="s">
+        <v>81</v>
+      </c>
+      <c r="L9">
+        <v>204260</v>
+      </c>
       <c r="M9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="J10" t="s">
+        <v>75</v>
+      </c>
+      <c r="N9" s="2">
+        <v>46935</v>
+      </c>
+      <c r="O9" s="3">
+        <v>2.3020833333333334E-2</v>
+      </c>
+      <c r="P9" s="3">
+        <v>7.7719907407407404E-2</v>
+      </c>
+      <c r="Q9">
+        <v>330</v>
+      </c>
+      <c r="R9">
+        <v>5244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="L10" t="s">
+      <c r="F10" t="s">
         <v>40</v>
       </c>
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" t="s">
+        <v>82</v>
+      </c>
+      <c r="L10">
+        <v>204258</v>
+      </c>
       <c r="M10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="J11" t="s">
+        <v>75</v>
+      </c>
+      <c r="N10" s="2">
+        <v>46935</v>
+      </c>
+      <c r="O10" s="3">
+        <v>2.2893518518518521E-2</v>
+      </c>
+      <c r="P10" s="3">
+        <v>7.8414351851851846E-2</v>
+      </c>
+      <c r="Q10">
+        <v>330</v>
+      </c>
+      <c r="R10">
+        <v>5244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="L11" t="s">
+      <c r="F11" t="s">
         <v>41</v>
       </c>
-      <c r="M11" t="s">
+      <c r="G11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="J12" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
         <v>13</v>
       </c>
-      <c r="L12" t="s">
+      <c r="F12" t="s">
         <v>42</v>
       </c>
-      <c r="M12" t="s">
+      <c r="G12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="J13" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
         <v>14</v>
       </c>
-      <c r="L13" t="s">
+      <c r="F13" t="s">
         <v>43</v>
       </c>
-      <c r="M13" t="s">
+      <c r="G13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="J14" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D14" t="s">
         <v>15</v>
       </c>
-      <c r="L14" t="s">
+      <c r="F14" t="s">
         <v>44</v>
       </c>
-      <c r="M14" t="s">
+      <c r="G14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="J15" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D15" t="s">
         <v>16</v>
       </c>
-      <c r="L15" t="s">
+      <c r="F15" t="s">
         <v>45</v>
       </c>
-      <c r="M15" t="s">
+      <c r="G15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="J16" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
         <v>17</v>
       </c>
-      <c r="L16" t="s">
+      <c r="F16" t="s">
         <v>46</v>
       </c>
-      <c r="M16" t="s">
+      <c r="G16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J17" t="s">
+    <row r="17" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D17" t="s">
         <v>18</v>
       </c>
-      <c r="L17" t="s">
+      <c r="F17" t="s">
         <v>47</v>
       </c>
-      <c r="M17" t="s">
+      <c r="G17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J18" t="s">
+    <row r="18" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
         <v>19</v>
       </c>
-      <c r="L18" t="s">
+      <c r="F18" t="s">
         <v>48</v>
       </c>
-      <c r="M18" t="s">
+      <c r="G18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J19" t="s">
+    <row r="19" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D19" t="s">
         <v>20</v>
       </c>
-      <c r="L19" t="s">
+      <c r="F19" t="s">
         <v>49</v>
       </c>
-      <c r="M19" t="s">
+      <c r="G19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J20" t="s">
+    <row r="20" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="L20" t="s">
+      <c r="F20" t="s">
         <v>50</v>
       </c>
-      <c r="M20" t="s">
+      <c r="G20" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J21" t="s">
+    <row r="21" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D21" t="s">
         <v>22</v>
       </c>
-      <c r="L21" t="s">
+      <c r="F21" t="s">
         <v>51</v>
       </c>
-      <c r="M21" t="s">
+      <c r="G21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J22" t="s">
+    <row r="22" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D22" t="s">
         <v>23</v>
       </c>
-      <c r="L22" t="s">
+      <c r="F22" t="s">
         <v>52</v>
       </c>
-      <c r="M22" t="s">
+      <c r="G22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J23" t="s">
+    <row r="23" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D23" t="s">
         <v>24</v>
       </c>
-      <c r="L23" t="s">
+      <c r="F23" t="s">
         <v>53</v>
       </c>
-      <c r="M23" t="s">
+      <c r="G23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J24" t="s">
+    <row r="24" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D24" t="s">
         <v>25</v>
       </c>
-      <c r="L24" t="s">
+      <c r="F24" t="s">
         <v>54</v>
       </c>
-      <c r="M24" t="s">
+      <c r="G24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J25" t="s">
+    <row r="25" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D25" t="s">
         <v>26</v>
       </c>
-      <c r="L25" t="s">
+      <c r="F25" t="s">
         <v>55</v>
       </c>
-      <c r="M25" t="s">
+      <c r="G25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J26" t="s">
+    <row r="26" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D26" t="s">
         <v>27</v>
       </c>
-      <c r="L26" t="s">
+      <c r="F26" t="s">
         <v>56</v>
       </c>
-      <c r="M26" t="s">
+      <c r="G26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J27" t="s">
+    <row r="27" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D27" t="s">
         <v>28</v>
       </c>
-      <c r="L27" t="s">
+      <c r="F27" t="s">
         <v>57</v>
       </c>
-      <c r="M27" t="s">
+      <c r="G27" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J28" t="s">
+    <row r="28" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D28" t="s">
         <v>29</v>
       </c>
-      <c r="L28" t="s">
+      <c r="F28" t="s">
         <v>58</v>
       </c>
-      <c r="M28" t="s">
+      <c r="G28" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J29" t="s">
+    <row r="29" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D29" t="s">
         <v>30</v>
       </c>
-      <c r="L29" t="s">
+      <c r="F29" t="s">
         <v>59</v>
       </c>
-      <c r="M29" t="s">
+      <c r="G29" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J30" t="s">
+    <row r="30" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="D30" t="s">
         <v>31</v>
       </c>
-      <c r="L30" t="s">
+      <c r="F30" t="s">
         <v>60</v>
       </c>
-      <c r="M30" t="s">
+      <c r="G30" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>